<commit_message>
Completed excel data import + data sheets
</commit_message>
<xml_diff>
--- a/Adventurers-Inc/Assets/Data/Classes/LevelInfo_Classes.xlsx
+++ b/Adventurers-Inc/Assets/Data/Classes/LevelInfo_Classes.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AIncorvaia\Dropbox\GameProjects\AdventurersInc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Dropbox\GameProjects\AdventurersInc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
     <sheet name="hunter" sheetId="8" r:id="rId4"/>
     <sheet name="merchant" sheetId="9" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,9 +51,6 @@
     <t>minDexterity</t>
   </si>
   <si>
-    <t>maxDetxerity</t>
-  </si>
-  <si>
     <t>minIntelligence</t>
   </si>
   <si>
@@ -65,11 +62,14 @@
   <si>
     <t>maxCharisma</t>
   </si>
+  <si>
+    <t>maxDexterity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -398,7 +398,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,19 +429,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -569,7 +569,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,19 +600,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -740,7 +740,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,19 +771,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -911,7 +911,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,19 +942,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1081,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,19 +1113,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>